<commit_message>
Regenerated example output for v3.2
</commit_message>
<xml_diff>
--- a/example/OUTPUTS/regulons/miniexExample_rankedRegulons.xlsx
+++ b/example/OUTPUTS/regulons/miniexExample_rankedRegulons.xlsx
@@ -1202,7 +1202,7 @@
         <v>0.001255994519296643</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0002618147807570945</v>
+        <v>0.0002618147807570943</v>
       </c>
       <c r="O9" t="n">
         <v>4.953195534546801</v>
@@ -1374,7 +1374,7 @@
         <v>0.001255994519296643</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0002618147807570945</v>
+        <v>0.0002618147807570943</v>
       </c>
       <c r="O11" t="n">
         <v>3.083898715393741</v>
@@ -1798,7 +1798,7 @@
         <v>1.49283e-27</v>
       </c>
       <c r="L16" t="n">
-        <v>0.7168949771689497</v>
+        <v>0.7168949771689498</v>
       </c>
       <c r="M16" t="n">
         <v>1.006849315068493</v>
@@ -2056,7 +2056,7 @@
         <v>6.816e-14</v>
       </c>
       <c r="L19" t="n">
-        <v>0.670391061452514</v>
+        <v>0.6703910614525139</v>
       </c>
       <c r="M19" t="n">
         <v>1.005586592178771</v>
@@ -2234,7 +2234,7 @@
         <v>0.00162540467203095</v>
       </c>
       <c r="N21" t="n">
-        <v>0.0002980234739537232</v>
+        <v>0.0002980234739537239</v>
       </c>
       <c r="O21" t="n">
         <v>4.639062478895823</v>
@@ -2406,7 +2406,7 @@
         <v>0.001726992464032884</v>
       </c>
       <c r="N23" t="n">
-        <v>0.000488938375135641</v>
+        <v>0.0004889383751356407</v>
       </c>
       <c r="O23" t="n">
         <v>0.6261123475065715</v>
@@ -2490,7 +2490,7 @@
         <v>0.00162540467203095</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0002980234739537232</v>
+        <v>0.0002980234739537239</v>
       </c>
       <c r="O24" t="n">
         <v>3.016939942683784</v>
@@ -2574,7 +2574,7 @@
         <v>0.001842125294968409</v>
       </c>
       <c r="N25" t="n">
-        <v>0.0004312178502940443</v>
+        <v>0.000431217850294044</v>
       </c>
       <c r="O25" t="n">
         <v>0.2392239606224263</v>
@@ -2658,7 +2658,7 @@
         <v>0.001726992464032884</v>
       </c>
       <c r="N26" t="n">
-        <v>0.000488938375135641</v>
+        <v>0.0004889383751356407</v>
       </c>
       <c r="O26" t="n">
         <v>0.4771769282296973</v>
@@ -2744,7 +2744,7 @@
         <v>0.00162540467203095</v>
       </c>
       <c r="N27" t="n">
-        <v>0.0001426181553480795</v>
+        <v>0.0001426181553480793</v>
       </c>
       <c r="O27" t="n">
         <v>1.599768904991229</v>
@@ -2822,7 +2822,7 @@
         <v>8.586150000000001e-06</v>
       </c>
       <c r="L28" t="n">
-        <v>0.4066985645933014</v>
+        <v>0.4066985645933015</v>
       </c>
       <c r="M28" t="n">
         <v>1.004784688995215</v>
@@ -3086,7 +3086,7 @@
         <v>0.001255994519296643</v>
       </c>
       <c r="N31" t="n">
-        <v>0.0002618147807570945</v>
+        <v>0.0002618147807570943</v>
       </c>
       <c r="O31" t="n">
         <v>3.033493712312571</v>
@@ -3344,7 +3344,7 @@
         <v>0.001381593971226307</v>
       </c>
       <c r="N34" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O34" t="n">
         <v>1.183980009831993</v>
@@ -3428,7 +3428,7 @@
         <v>0.00162540467203095</v>
       </c>
       <c r="N35" t="n">
-        <v>0.0002980234739537232</v>
+        <v>0.0002980234739537239</v>
       </c>
       <c r="O35" t="n">
         <v>0.9248081598275221</v>
@@ -3598,7 +3598,7 @@
         <v>0.001842125294968409</v>
       </c>
       <c r="N37" t="n">
-        <v>0.0004312178502940443</v>
+        <v>0.000431217850294044</v>
       </c>
       <c r="O37" t="n">
         <v>0.2110572766332232</v>
@@ -3682,7 +3682,7 @@
         <v>0.001842125294968409</v>
       </c>
       <c r="N38" t="n">
-        <v>0.0001605746509971327</v>
+        <v>0.0001605746509971325</v>
       </c>
       <c r="O38" t="n">
         <v>0.5396664433679511</v>
@@ -3766,7 +3766,7 @@
         <v>0.001381593971226307</v>
       </c>
       <c r="N39" t="n">
-        <v>0.0002032090869488327</v>
+        <v>0.0002032090869488329</v>
       </c>
       <c r="O39" t="n">
         <v>0.2810383621681332</v>
@@ -3850,7 +3850,7 @@
         <v>0.001381593971226307</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O40" t="n">
         <v>1.033251522534279</v>
@@ -4018,7 +4018,7 @@
         <v>0.001381593971226307</v>
       </c>
       <c r="N42" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O42" t="n">
         <v>1.10280973904715</v>
@@ -4098,7 +4098,7 @@
         <v>0.001842125294968409</v>
       </c>
       <c r="N43" t="n">
-        <v>0.0001605746509971327</v>
+        <v>0.0001605746509971325</v>
       </c>
       <c r="O43" t="n">
         <v>0.3804760304538707</v>
@@ -4182,7 +4182,7 @@
         <v>0.001842125294968409</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0004312178502940443</v>
+        <v>0.000431217850294044</v>
       </c>
       <c r="O44" t="n">
         <v>0.7263413045662546</v>
@@ -4266,7 +4266,7 @@
         <v>0.001381593971226307</v>
       </c>
       <c r="N45" t="n">
-        <v>0.0002032090869488327</v>
+        <v>0.0002032090869488329</v>
       </c>
       <c r="O45" t="n">
         <v>0.30469016477851</v>
@@ -4344,13 +4344,13 @@
         <v>2.15774e-07</v>
       </c>
       <c r="L46" t="n">
-        <v>0.7101449275362318</v>
+        <v>0.7101449275362319</v>
       </c>
       <c r="M46" t="n">
         <v>0.001381593971226307</v>
       </c>
       <c r="N46" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O46" t="n">
         <v>0.7743537907372691</v>
@@ -4428,13 +4428,13 @@
         <v>6.902279999999998e-13</v>
       </c>
       <c r="L47" t="n">
-        <v>0.619718309859155</v>
+        <v>0.6197183098591549</v>
       </c>
       <c r="M47" t="n">
         <v>0.001255994519296643</v>
       </c>
       <c r="N47" t="n">
-        <v>0.0002618147807570945</v>
+        <v>0.0002618147807570943</v>
       </c>
       <c r="O47" t="n">
         <v>0.65374744862436</v>
@@ -4512,13 +4512,13 @@
         <v>0.000448189</v>
       </c>
       <c r="L48" t="n">
-        <v>0.5681818181818181</v>
+        <v>0.5681818181818182</v>
       </c>
       <c r="M48" t="n">
         <v>0.001381593971226307</v>
       </c>
       <c r="N48" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O48" t="n">
         <v>0.8741717789020859</v>
@@ -4596,13 +4596,13 @@
         <v>4.39481e-12</v>
       </c>
       <c r="L49" t="n">
-        <v>0.7042253521126761</v>
+        <v>0.7042253521126759</v>
       </c>
       <c r="M49" t="n">
         <v>0.001381593971226307</v>
       </c>
       <c r="N49" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O49" t="n">
         <v>0.5059462670765771</v>
@@ -4686,7 +4686,7 @@
         <v>0.001973705673180439</v>
       </c>
       <c r="N50" t="n">
-        <v>0.0001055677946906507</v>
+        <v>0.0001055677946906508</v>
       </c>
       <c r="O50" t="n">
         <v>2.080360826732798</v>
@@ -4766,7 +4766,7 @@
         <v>0.001381593971226307</v>
       </c>
       <c r="N51" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O51" t="n">
         <v>0.2159517637420749</v>
@@ -4850,7 +4850,7 @@
         <v>0.001381593971226307</v>
       </c>
       <c r="N52" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O52" t="n">
         <v>0.5859301537285536</v>
@@ -4934,7 +4934,7 @@
         <v>0.001381593971226307</v>
       </c>
       <c r="N53" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O53" t="n">
         <v>0.2497211155089533</v>
@@ -5018,7 +5018,7 @@
         <v>0.001381593971226307</v>
       </c>
       <c r="N54" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O54" t="n">
         <v>0.6151389349457237</v>
@@ -5102,7 +5102,7 @@
         <v>0.001255994519296643</v>
       </c>
       <c r="N55" t="n">
-        <v>0.0002618147807570945</v>
+        <v>0.0002618147807570943</v>
       </c>
       <c r="O55" t="n">
         <v>0.5057668037080942</v>
@@ -5186,7 +5186,7 @@
         <v>0.001381593971226307</v>
       </c>
       <c r="N56" t="n">
-        <v>0.0003352638902046453</v>
+        <v>0.0003352638902046445</v>
       </c>
       <c r="O56" t="n">
         <v>0.1856115106002673</v>
@@ -5270,7 +5270,7 @@
         <v>0.001973705673180439</v>
       </c>
       <c r="N57" t="n">
-        <v>0.0001055677946906507</v>
+        <v>0.0001055677946906508</v>
       </c>
       <c r="O57" t="n">
         <v>0.6942540664004011</v>
@@ -5348,13 +5348,13 @@
         <v>4.23325e-08</v>
       </c>
       <c r="L58" t="n">
-        <v>0.4615384615384615</v>
+        <v>0.4615384615384616</v>
       </c>
       <c r="M58" t="n">
         <v>0.00162540467203095</v>
       </c>
       <c r="N58" t="n">
-        <v>0.0001426181553480795</v>
+        <v>0.0001426181553480793</v>
       </c>
       <c r="O58" t="n">
         <v>0.5661667093636524</v>
@@ -5438,7 +5438,7 @@
         <v>0.001842125294968409</v>
       </c>
       <c r="N59" t="n">
-        <v>0.0001605746509971327</v>
+        <v>0.0001605746509971325</v>
       </c>
       <c r="O59" t="n">
         <v>0.6155367993531059</v>
@@ -5516,13 +5516,13 @@
         <v>2.96494e-08</v>
       </c>
       <c r="L60" t="n">
-        <v>0.3045454545454545</v>
+        <v>0.3045454545454546</v>
       </c>
       <c r="M60" t="n">
         <v>0.001973705673180439</v>
       </c>
       <c r="N60" t="n">
-        <v>0.0001055677946906507</v>
+        <v>0.0001055677946906508</v>
       </c>
       <c r="O60" t="n">
         <v>0.1899870412725211</v>
@@ -5606,7 +5606,7 @@
         <v>0.001973705673180439</v>
       </c>
       <c r="N61" t="n">
-        <v>0.0001055677946906507</v>
+        <v>0.0001055677946906508</v>
       </c>
       <c r="O61" t="n">
         <v>0.3808292199904637</v>

</xml_diff>